<commit_message>
Hægt er að fylla út í töflu
</commit_message>
<xml_diff>
--- a/Testgögn.xlsx
+++ b/Testgögn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjorn\PycharmProjects\Thrifalisti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B22ABF0-1658-4632-B0D3-9BDE6EDC9572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC8E06-1C01-48BF-91CF-942CFE24548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="100">
   <si>
     <t xml:space="preserve"> Rauða hús 2.-3. bekkur</t>
   </si>
@@ -1447,7 +1447,7 @@
   <dimension ref="A1:AMJ99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -1542,7 +1542,9 @@
         <v>9</v>
       </c>
       <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="C6" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>

</xml_diff>